<commit_message>
new file for arpt
</commit_message>
<xml_diff>
--- a/revenue_per_city.xlsx
+++ b/revenue_per_city.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marag\Documents\arr-travel-partners-predictor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marag\Documents\Hotels-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90CD192-E76C-4F1F-B5A7-97029E352E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2938585-0F93-46D6-9D19-4EB9BC5F0219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="288">
   <si>
     <t>abu dhabi</t>
   </si>
@@ -820,12 +820,84 @@
   </si>
   <si>
     <t>wroclaw</t>
+  </si>
+  <si>
+    <t>adelaide</t>
+  </si>
+  <si>
+    <t>almaty</t>
+  </si>
+  <si>
+    <t>bahrain</t>
+  </si>
+  <si>
+    <t>bangalore</t>
+  </si>
+  <si>
+    <t>biarritz</t>
+  </si>
+  <si>
+    <t>calgary</t>
+  </si>
+  <si>
+    <t>chisinau</t>
+  </si>
+  <si>
+    <t>dhaka</t>
+  </si>
+  <si>
+    <t>djerba</t>
+  </si>
+  <si>
+    <t>eindhoven</t>
+  </si>
+  <si>
+    <t>fes</t>
+  </si>
+  <si>
+    <t>honolulu</t>
+  </si>
+  <si>
+    <t>kuwait city</t>
+  </si>
+  <si>
+    <t>la paz</t>
+  </si>
+  <si>
+    <t>lagos</t>
+  </si>
+  <si>
+    <t>mendoza</t>
+  </si>
+  <si>
+    <t>nadi</t>
+  </si>
+  <si>
+    <t>phoenix</t>
+  </si>
+  <si>
+    <t>porto alegre</t>
+  </si>
+  <si>
+    <t>rabat</t>
+  </si>
+  <si>
+    <t>san jose (ca)</t>
+  </si>
+  <si>
+    <t>toronto</t>
+  </si>
+  <si>
+    <t>tunis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00;\-&quot;€&quot;\ #,##0.00;&quot;€&quot;\ #,##0.00"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -862,16 +934,16 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00;\-&quot;€&quot;\ #,##0.00;&quot;€&quot;\ #,##0.00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -887,8 +959,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B265">
-  <autoFilter ref="A1:B265" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B288">
+  <autoFilter ref="A1:B288" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="city_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="revenue_per_city" dataDxfId="0"/>
@@ -1194,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B265"/>
+  <dimension ref="A1:B288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
-      <selection activeCell="F261" sqref="F261"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G277" sqref="G277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1214,2109 +1286,2293 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>16.054829545454552</v>
+      <c r="B2" s="2">
+        <v>16.770018170805564</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>213</v>
       </c>
-      <c r="B3" s="1">
-        <v>9.9000000000000021</v>
+      <c r="B3" s="2">
+        <v>10.622222222222222</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>214</v>
-      </c>
-      <c r="B4" s="1">
-        <v>9.0752808988763931</v>
+        <v>265</v>
+      </c>
+      <c r="B4" s="2">
+        <v>36.266666666666659</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1">
-        <v>22.930399313009989</v>
+        <v>214</v>
+      </c>
+      <c r="B5" s="2">
+        <v>9.3654471544715587</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>215</v>
-      </c>
-      <c r="B6" s="1">
-        <v>16.110204081632645</v>
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>25.747621621621672</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>13.25363825363825</v>
+        <v>266</v>
+      </c>
+      <c r="B7" s="2">
+        <v>12.049999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1">
-        <v>22.468352788583434</v>
+        <v>215</v>
+      </c>
+      <c r="B8" s="2">
+        <v>16.348076923076928</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>216</v>
-      </c>
-      <c r="B9" s="1">
-        <v>12.564705882352946</v>
+        <v>2</v>
+      </c>
+      <c r="B9" s="2">
+        <v>14.369966442953011</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1">
-        <v>14.711225225224752</v>
+        <v>3</v>
+      </c>
+      <c r="B10" s="2">
+        <v>22.846333333331625</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1">
-        <v>16.836986301369887</v>
+        <v>216</v>
+      </c>
+      <c r="B11" s="2">
+        <v>12.210526315789467</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="1">
-        <v>16.853546099290377</v>
+        <v>4</v>
+      </c>
+      <c r="B12" s="2">
+        <v>15.192422745872527</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="1">
-        <v>13.815999999999992</v>
+        <v>5</v>
+      </c>
+      <c r="B13" s="2">
+        <v>17.334355828220883</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>217</v>
-      </c>
-      <c r="B14" s="1">
-        <v>15.399999999999999</v>
+        <v>6</v>
+      </c>
+      <c r="B14" s="2">
+        <v>17.073490427098385</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="1">
-        <v>19.76358397019651</v>
+        <v>7</v>
+      </c>
+      <c r="B15" s="2">
+        <v>15.342857142857138</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="1">
-        <v>28.846153846153875</v>
+        <v>217</v>
+      </c>
+      <c r="B16" s="2">
+        <v>12.06</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>218</v>
-      </c>
-      <c r="B17" s="1">
-        <v>21.388888888888886</v>
+        <v>8</v>
+      </c>
+      <c r="B17" s="2">
+        <v>20.472004262994268</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="1">
-        <v>33.441935483870935</v>
+        <v>9</v>
+      </c>
+      <c r="B18" s="2">
+        <v>33.335754189944119</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="1">
-        <v>6.4700598802395426</v>
+        <v>218</v>
+      </c>
+      <c r="B19" s="2">
+        <v>53.838461538461551</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="1">
-        <v>8.6317626006553443</v>
+        <v>10</v>
+      </c>
+      <c r="B20" s="2">
+        <v>43.479569892473101</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>219</v>
-      </c>
-      <c r="B21" s="1">
-        <v>36.950000000000003</v>
+        <v>267</v>
+      </c>
+      <c r="B21" s="2">
+        <v>42.933333333333344</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="1">
-        <v>8.8293241229849908</v>
+        <v>11</v>
+      </c>
+      <c r="B22" s="2">
+        <v>7.5639484978540636</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="1">
-        <v>22.635372848948283</v>
+        <v>12</v>
+      </c>
+      <c r="B23" s="2">
+        <v>8.9445964107829106</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="1">
-        <v>16.596254126416959</v>
+        <v>219</v>
+      </c>
+      <c r="B24" s="2">
+        <v>63.21764705882353</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="1">
-        <v>23.877208480565351</v>
+        <v>268</v>
+      </c>
+      <c r="B25" s="2">
+        <v>16.181666666666665</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="1">
-        <v>30.133170731707384</v>
+        <v>13</v>
+      </c>
+      <c r="B26" s="2">
+        <v>9.1170720076297691</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>220</v>
-      </c>
-      <c r="B27" s="1">
-        <v>5.1000000000000014</v>
+        <v>14</v>
+      </c>
+      <c r="B27" s="2">
+        <v>23.051051051050965</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="1">
-        <v>16.538624338624302</v>
+        <v>15</v>
+      </c>
+      <c r="B28" s="2">
+        <v>16.956022629979188</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="1">
-        <v>11.761727821644044</v>
+        <v>16</v>
+      </c>
+      <c r="B29" s="2">
+        <v>23.99607843137251</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>221</v>
-      </c>
-      <c r="B30" s="1">
-        <v>12.177251184834169</v>
+        <v>17</v>
+      </c>
+      <c r="B30" s="2">
+        <v>36.896391752577323</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="1">
-        <v>24.592666666666663</v>
+        <v>220</v>
+      </c>
+      <c r="B31" s="2">
+        <v>12.818181818181818</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="1">
-        <v>20.141724866003283</v>
+        <v>18</v>
+      </c>
+      <c r="B32" s="2">
+        <v>16.350168350168239</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="1">
-        <v>22.186655112651636</v>
+        <v>19</v>
+      </c>
+      <c r="B33" s="2">
+        <v>12.007032793362143</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>222</v>
-      </c>
-      <c r="B34" s="1">
-        <v>30.557142857142857</v>
+        <v>221</v>
+      </c>
+      <c r="B34" s="2">
+        <v>13.457680250783733</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="1">
-        <v>14.549853085210479</v>
+        <v>20</v>
+      </c>
+      <c r="B35" s="2">
+        <v>34.415248226950347</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>24</v>
-      </c>
-      <c r="B36" s="1">
-        <v>7.1275648949319708</v>
+        <v>21</v>
+      </c>
+      <c r="B36" s="2">
+        <v>20.774766159428275</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>25</v>
-      </c>
-      <c r="B37" s="1">
-        <v>28.683650793650756</v>
+        <v>269</v>
+      </c>
+      <c r="B37" s="2">
+        <v>46.509302325581395</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="1">
-        <v>26.824661246612262</v>
+        <v>22</v>
+      </c>
+      <c r="B38" s="2">
+        <v>22.043767186067701</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>27</v>
-      </c>
-      <c r="B39" s="1">
-        <v>35.094845360824777</v>
+        <v>222</v>
+      </c>
+      <c r="B39" s="2">
+        <v>51.601666666666674</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>28</v>
-      </c>
-      <c r="B40" s="1">
-        <v>10.796428571428574</v>
+        <v>23</v>
+      </c>
+      <c r="B40" s="2">
+        <v>15.301683381088681</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>29</v>
-      </c>
-      <c r="B41" s="1">
-        <v>25.401515151515184</v>
+        <v>24</v>
+      </c>
+      <c r="B41" s="2">
+        <v>7.7247810858142767</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>223</v>
-      </c>
-      <c r="B42" s="1">
-        <v>37.849999999999994</v>
+        <v>25</v>
+      </c>
+      <c r="B42" s="2">
+        <v>28.342937853107365</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>30</v>
-      </c>
-      <c r="B43" s="1">
-        <v>21.979496992892592</v>
+        <v>26</v>
+      </c>
+      <c r="B43" s="2">
+        <v>28.13365487674151</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>31</v>
-      </c>
-      <c r="B44" s="1">
-        <v>12.170579813886704</v>
+        <v>27</v>
+      </c>
+      <c r="B44" s="2">
+        <v>35.348550724637711</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>32</v>
-      </c>
-      <c r="B45" s="1">
-        <v>13.959755723629527</v>
+        <v>28</v>
+      </c>
+      <c r="B45" s="2">
+        <v>10.708316831683151</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>33</v>
-      </c>
-      <c r="B46" s="1">
-        <v>14.295021200930799</v>
+        <v>29</v>
+      </c>
+      <c r="B46" s="2">
+        <v>32.844600938967176</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>224</v>
-      </c>
-      <c r="B47" s="1">
-        <v>14.933333333333332</v>
+        <v>223</v>
+      </c>
+      <c r="B47" s="2">
+        <v>40.446428571428569</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="1">
-        <v>26.236125273124422</v>
+        <v>30</v>
+      </c>
+      <c r="B48" s="2">
+        <v>22.171405859641261</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>35</v>
-      </c>
-      <c r="B49" s="1">
-        <v>24.300952380952413</v>
+        <v>31</v>
+      </c>
+      <c r="B49" s="2">
+        <v>12.406683322922918</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>36</v>
-      </c>
-      <c r="B50" s="1">
-        <v>7.4884738527215813</v>
+        <v>32</v>
+      </c>
+      <c r="B50" s="2">
+        <v>14.159188188549514</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>37</v>
-      </c>
-      <c r="B51" s="1">
-        <v>10.243750000000002</v>
+        <v>33</v>
+      </c>
+      <c r="B51" s="2">
+        <v>14.806567564274832</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>38</v>
-      </c>
-      <c r="B52" s="1">
-        <v>17.878537492254271</v>
+        <v>224</v>
+      </c>
+      <c r="B52" s="2">
+        <v>14.17615384615384</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>39</v>
-      </c>
-      <c r="B53" s="1">
-        <v>13.171112748710621</v>
+        <v>34</v>
+      </c>
+      <c r="B53" s="2">
+        <v>26.736183790682777</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>40</v>
-      </c>
-      <c r="B54" s="1">
-        <v>14.985807291666577</v>
+        <v>35</v>
+      </c>
+      <c r="B54" s="2">
+        <v>24.560442260442283</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>41</v>
-      </c>
-      <c r="B55" s="1">
-        <v>8.1912162162162989</v>
+        <v>36</v>
+      </c>
+      <c r="B55" s="2">
+        <v>8.3096872284970527</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>42</v>
-      </c>
-      <c r="B56" s="1">
-        <v>10.314745403111571</v>
+        <v>270</v>
+      </c>
+      <c r="B56" s="2">
+        <v>23.090526315789479</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>43</v>
-      </c>
-      <c r="B57" s="1">
-        <v>30.884544557711646</v>
+        <v>37</v>
+      </c>
+      <c r="B57" s="2">
+        <v>10.741666666666667</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>44</v>
-      </c>
-      <c r="B58" s="1">
-        <v>11.894531249999995</v>
+        <v>38</v>
+      </c>
+      <c r="B58" s="2">
+        <v>18.319227661981209</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>45</v>
-      </c>
-      <c r="B59" s="1">
-        <v>4.9377510040160981</v>
+        <v>39</v>
+      </c>
+      <c r="B59" s="2">
+        <v>12.950766936514778</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>46</v>
-      </c>
-      <c r="B60" s="1">
-        <v>31.859574468085036</v>
+        <v>40</v>
+      </c>
+      <c r="B60" s="2">
+        <v>15.542636457260496</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>47</v>
-      </c>
-      <c r="B61" s="1">
-        <v>22.765486725663695</v>
+        <v>41</v>
+      </c>
+      <c r="B61" s="2">
+        <v>9.2286370597244201</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>48</v>
-      </c>
-      <c r="B62" s="1">
-        <v>10.925077399380674</v>
+        <v>42</v>
+      </c>
+      <c r="B62" s="2">
+        <v>10.61124849215912</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>49</v>
-      </c>
-      <c r="B63" s="1">
-        <v>31.648930481283841</v>
+        <v>43</v>
+      </c>
+      <c r="B63" s="2">
+        <v>32.493833333334088</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>50</v>
-      </c>
-      <c r="B64" s="1">
-        <v>20.603948707511766</v>
+        <v>44</v>
+      </c>
+      <c r="B64" s="2">
+        <v>12.182840236686378</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>51</v>
-      </c>
-      <c r="B65" s="1">
-        <v>12.248519520142954</v>
+        <v>45</v>
+      </c>
+      <c r="B65" s="2">
+        <v>5.7649122807017816</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>52</v>
-      </c>
-      <c r="B66" s="1">
-        <v>20.009324009323983</v>
+        <v>46</v>
+      </c>
+      <c r="B66" s="2">
+        <v>40.518316831683187</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>53</v>
-      </c>
-      <c r="B67" s="1">
-        <v>5.6877192982456046</v>
+        <v>271</v>
+      </c>
+      <c r="B67" s="2">
+        <v>16.873913043478261</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>54</v>
-      </c>
-      <c r="B68" s="1">
-        <v>18.100509626275098</v>
+        <v>47</v>
+      </c>
+      <c r="B68" s="2">
+        <v>23.937499999999968</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>55</v>
-      </c>
-      <c r="B69" s="1">
-        <v>4.6725714285714233</v>
+        <v>48</v>
+      </c>
+      <c r="B69" s="2">
+        <v>11.264243997404208</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>56</v>
-      </c>
-      <c r="B70" s="1">
-        <v>18.855072463768174</v>
+        <v>49</v>
+      </c>
+      <c r="B70" s="2">
+        <v>31.540497237569287</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>225</v>
-      </c>
-      <c r="B71" s="1">
-        <v>26.859259259259261</v>
+        <v>50</v>
+      </c>
+      <c r="B71" s="2">
+        <v>21.013297620924014</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>226</v>
-      </c>
-      <c r="B72" s="1">
-        <v>20.133333333333336</v>
+        <v>51</v>
+      </c>
+      <c r="B72" s="2">
+        <v>12.429895497071463</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>57</v>
-      </c>
-      <c r="B73" s="1">
-        <v>9.0773333333333301</v>
+        <v>52</v>
+      </c>
+      <c r="B73" s="2">
+        <v>21.120465890182995</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>58</v>
-      </c>
-      <c r="B74" s="1">
-        <v>13.718579234972722</v>
+        <v>53</v>
+      </c>
+      <c r="B74" s="2">
+        <v>5.7706484641638314</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>59</v>
-      </c>
-      <c r="B75" s="1">
-        <v>12.139744102360066</v>
+        <v>54</v>
+      </c>
+      <c r="B75" s="2">
+        <v>17.766025868179074</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>60</v>
-      </c>
-      <c r="B76" s="1">
-        <v>26.188843616607123</v>
+        <v>55</v>
+      </c>
+      <c r="B76" s="2">
+        <v>5.8363636363636315</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>61</v>
-      </c>
-      <c r="B77" s="1">
-        <v>10.217732855680776</v>
+        <v>56</v>
+      </c>
+      <c r="B77" s="2">
+        <v>19.752711640211686</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>62</v>
-      </c>
-      <c r="B78" s="1">
-        <v>12.290526315789473</v>
+        <v>225</v>
+      </c>
+      <c r="B78" s="2">
+        <v>27.278260869565212</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>63</v>
-      </c>
-      <c r="B79" s="1">
-        <v>30.166985645933092</v>
+        <v>226</v>
+      </c>
+      <c r="B79" s="2">
+        <v>42.6235294117647</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>64</v>
-      </c>
-      <c r="B80" s="1">
-        <v>23.193497922267824</v>
+        <v>57</v>
+      </c>
+      <c r="B80" s="2">
+        <v>9.6907317073170773</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>65</v>
-      </c>
-      <c r="B81" s="1">
-        <v>25.547539124518977</v>
+        <v>272</v>
+      </c>
+      <c r="B81" s="2">
+        <v>26.400000000000002</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>66</v>
-      </c>
-      <c r="B82" s="1">
-        <v>38.071818710052256</v>
+        <v>273</v>
+      </c>
+      <c r="B82" s="2">
+        <v>20.18888888888889</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>67</v>
-      </c>
-      <c r="B83" s="1">
-        <v>11.816666666666665</v>
+        <v>58</v>
+      </c>
+      <c r="B83" s="2">
+        <v>18.608764940239197</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>68</v>
-      </c>
-      <c r="B84" s="1">
-        <v>27.072745831915363</v>
+        <v>59</v>
+      </c>
+      <c r="B84" s="2">
+        <v>12.601550569717386</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>69</v>
-      </c>
-      <c r="B85" s="1">
-        <v>9.968138195777362</v>
+        <v>60</v>
+      </c>
+      <c r="B85" s="2">
+        <v>27.177272727271781</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>227</v>
-      </c>
-      <c r="B86" s="1">
-        <v>32.946031746031743</v>
+        <v>61</v>
+      </c>
+      <c r="B86" s="2">
+        <v>10.544549763033359</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>228</v>
-      </c>
-      <c r="B87" s="1">
-        <v>22.707777777777775</v>
+        <v>62</v>
+      </c>
+      <c r="B87" s="2">
+        <v>11.781967213114752</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>70</v>
-      </c>
-      <c r="B88" s="1">
-        <v>19.057757009345703</v>
+        <v>63</v>
+      </c>
+      <c r="B88" s="2">
+        <v>30.010410958904188</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>229</v>
-      </c>
-      <c r="B89" s="1">
-        <v>7.3285714285714301</v>
+        <v>64</v>
+      </c>
+      <c r="B89" s="2">
+        <v>23.230794962612805</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>230</v>
-      </c>
-      <c r="B90" s="1">
-        <v>34.219999999999985</v>
+        <v>274</v>
+      </c>
+      <c r="B90" s="2">
+        <v>67.150000000000006</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>71</v>
-      </c>
-      <c r="B91" s="1">
-        <v>18.91822615056422</v>
+        <v>65</v>
+      </c>
+      <c r="B91" s="2">
+        <v>25.194238475005161</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>72</v>
-      </c>
-      <c r="B92" s="1">
-        <v>12.945136612021923</v>
+        <v>275</v>
+      </c>
+      <c r="B92" s="2">
+        <v>8.1374999999999993</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>73</v>
-      </c>
-      <c r="B93" s="1">
-        <v>15.286842105263124</v>
+        <v>66</v>
+      </c>
+      <c r="B93" s="2">
+        <v>40.4581628714784</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>231</v>
-      </c>
-      <c r="B94" s="1">
-        <v>20</v>
+        <v>67</v>
+      </c>
+      <c r="B94" s="2">
+        <v>10.693333333333332</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>74</v>
-      </c>
-      <c r="B95" s="1">
-        <v>17.008938547486014</v>
+        <v>68</v>
+      </c>
+      <c r="B95" s="2">
+        <v>27.507434320849587</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>75</v>
-      </c>
-      <c r="B96" s="1">
-        <v>25.488163265306113</v>
+        <v>69</v>
+      </c>
+      <c r="B96" s="2">
+        <v>11.0550847457627</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>76</v>
-      </c>
-      <c r="B97" s="1">
-        <v>6.9373188405796986</v>
+        <v>227</v>
+      </c>
+      <c r="B97" s="2">
+        <v>34.491443850267395</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>232</v>
-      </c>
-      <c r="B98" s="1">
-        <v>26.639999999999997</v>
+        <v>228</v>
+      </c>
+      <c r="B98" s="2">
+        <v>24.37008547008546</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>77</v>
-      </c>
-      <c r="B99" s="1">
-        <v>16.749059334297772</v>
+        <v>70</v>
+      </c>
+      <c r="B99" s="2">
+        <v>19.104930555555519</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>78</v>
-      </c>
-      <c r="B100" s="1">
-        <v>5.3759446315004462</v>
+        <v>229</v>
+      </c>
+      <c r="B100" s="2">
+        <v>14.701470588235303</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>79</v>
-      </c>
-      <c r="B101" s="1">
-        <v>16.868163265306066</v>
+        <v>230</v>
+      </c>
+      <c r="B101" s="2">
+        <v>34.450381679389324</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>80</v>
-      </c>
-      <c r="B102" s="1">
-        <v>30.131521739130449</v>
+        <v>71</v>
+      </c>
+      <c r="B102" s="2">
+        <v>19.835842803030811</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>81</v>
-      </c>
-      <c r="B103" s="1">
-        <v>5.7774330042312627</v>
+        <v>72</v>
+      </c>
+      <c r="B103" s="2">
+        <v>13.053729977116744</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>82</v>
-      </c>
-      <c r="B104" s="1">
-        <v>59.60857142857143</v>
+        <v>73</v>
+      </c>
+      <c r="B104" s="2">
+        <v>24.403436426116876</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>83</v>
-      </c>
-      <c r="B105" s="1">
-        <v>12.69073984358443</v>
+        <v>231</v>
+      </c>
+      <c r="B105" s="2">
+        <v>17.666666666666668</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>84</v>
-      </c>
-      <c r="B106" s="1">
-        <v>17.870541692026599</v>
+        <v>74</v>
+      </c>
+      <c r="B106" s="2">
+        <v>17.050377358490554</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>85</v>
-      </c>
-      <c r="B107" s="1">
-        <v>9.4643757159219177</v>
+        <v>75</v>
+      </c>
+      <c r="B107" s="2">
+        <v>26.40591133004926</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>86</v>
-      </c>
-      <c r="B108" s="1">
-        <v>18.930000000000014</v>
+        <v>76</v>
+      </c>
+      <c r="B108" s="2">
+        <v>7.349751518497996</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>87</v>
-      </c>
-      <c r="B109" s="1">
-        <v>13.680672268907584</v>
+        <v>232</v>
+      </c>
+      <c r="B109" s="2">
+        <v>30.701818181818179</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>233</v>
-      </c>
-      <c r="B110" s="1">
-        <v>20.25</v>
+        <v>77</v>
+      </c>
+      <c r="B110" s="2">
+        <v>17.424121405750455</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>88</v>
-      </c>
-      <c r="B111" s="1">
-        <v>5.7102272727272512</v>
+        <v>78</v>
+      </c>
+      <c r="B111" s="2">
+        <v>5.6946622734762764</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>234</v>
-      </c>
-      <c r="B112" s="1">
-        <v>18.880000000000003</v>
+        <v>79</v>
+      </c>
+      <c r="B112" s="2">
+        <v>16.877616747181925</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>89</v>
-      </c>
-      <c r="B113" s="1">
-        <v>18.922621902477758</v>
+        <v>276</v>
+      </c>
+      <c r="B113" s="2">
+        <v>45.000000000000036</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>90</v>
-      </c>
-      <c r="B114" s="1">
-        <v>6.9355681818182164</v>
+        <v>80</v>
+      </c>
+      <c r="B114" s="2">
+        <v>33.602952029520317</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>91</v>
-      </c>
-      <c r="B115" s="1">
-        <v>17.777174780526128</v>
+        <v>81</v>
+      </c>
+      <c r="B115" s="2">
+        <v>6.2039400665926214</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>92</v>
-      </c>
-      <c r="B116" s="1">
-        <v>5.2867924528301913</v>
+        <v>82</v>
+      </c>
+      <c r="B116" s="2">
+        <v>39.353333333333339</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>93</v>
-      </c>
-      <c r="B117" s="1">
-        <v>7.4118623962041044</v>
+        <v>83</v>
+      </c>
+      <c r="B117" s="2">
+        <v>12.983350351545226</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>94</v>
-      </c>
-      <c r="B118" s="1">
-        <v>10.994391025640734</v>
+        <v>84</v>
+      </c>
+      <c r="B118" s="2">
+        <v>18.700932504440299</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>95</v>
-      </c>
-      <c r="B119" s="1">
-        <v>8.3272333848530788</v>
+        <v>85</v>
+      </c>
+      <c r="B119" s="2">
+        <v>9.5738489871085282</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>96</v>
-      </c>
-      <c r="B120" s="1">
-        <v>4.9744966442952929</v>
+        <v>86</v>
+      </c>
+      <c r="B120" s="2">
+        <v>25.673333333333328</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>97</v>
-      </c>
-      <c r="B121" s="1">
-        <v>17.297459165154205</v>
+        <v>87</v>
+      </c>
+      <c r="B121" s="2">
+        <v>13.859018404907962</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>98</v>
-      </c>
-      <c r="B122" s="1">
-        <v>11.181210191082764</v>
+        <v>233</v>
+      </c>
+      <c r="B122" s="2">
+        <v>21.76235294117647</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>235</v>
-      </c>
-      <c r="B123" s="1">
-        <v>25.12857142857143</v>
+        <v>88</v>
+      </c>
+      <c r="B123" s="2">
+        <v>5.8074418604651008</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>236</v>
-      </c>
-      <c r="B124" s="1">
-        <v>31.822222222222219</v>
+        <v>234</v>
+      </c>
+      <c r="B124" s="2">
+        <v>19.940909090909091</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>99</v>
-      </c>
-      <c r="B125" s="1">
-        <v>10.371453437772047</v>
+        <v>89</v>
+      </c>
+      <c r="B125" s="2">
+        <v>18.48961180973183</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>100</v>
-      </c>
-      <c r="B126" s="1">
-        <v>17.358664126827936</v>
+        <v>90</v>
+      </c>
+      <c r="B126" s="2">
+        <v>7.2835664335664649</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>101</v>
-      </c>
-      <c r="B127" s="1">
-        <v>23.228571428571453</v>
+        <v>91</v>
+      </c>
+      <c r="B127" s="2">
+        <v>18.050980810234091</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>102</v>
-      </c>
-      <c r="B128" s="1">
-        <v>14.13741444866907</v>
+        <v>92</v>
+      </c>
+      <c r="B128" s="2">
+        <v>5.7681415929203599</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>237</v>
-      </c>
-      <c r="B129" s="1">
-        <v>10.3</v>
+        <v>93</v>
+      </c>
+      <c r="B129" s="2">
+        <v>7.8305801376598492</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>103</v>
-      </c>
-      <c r="B130" s="1">
-        <v>33.151938601477703</v>
+        <v>94</v>
+      </c>
+      <c r="B130" s="2">
+        <v>11.393815118598747</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>238</v>
-      </c>
-      <c r="B131" s="1">
-        <v>29.800000000000004</v>
+        <v>95</v>
+      </c>
+      <c r="B131" s="2">
+        <v>8.7348323576369911</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>104</v>
-      </c>
-      <c r="B132" s="1">
-        <v>23.044414168937312</v>
+        <v>277</v>
+      </c>
+      <c r="B132" s="2">
+        <v>34.13333333333334</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>105</v>
-      </c>
-      <c r="B133" s="1">
-        <v>6.301149425287365</v>
+        <v>278</v>
+      </c>
+      <c r="B133" s="2">
+        <v>6.1999999999999993</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>106</v>
-      </c>
-      <c r="B134" s="1">
-        <v>26.190855263157658</v>
+        <v>279</v>
+      </c>
+      <c r="B134" s="2">
+        <v>18.327272727272724</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>107</v>
-      </c>
-      <c r="B135" s="1">
-        <v>12.859741935483852</v>
+        <v>96</v>
+      </c>
+      <c r="B135" s="2">
+        <v>5.3467213114753998</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>239</v>
-      </c>
-      <c r="B136" s="1">
-        <v>15.963636363636363</v>
+        <v>97</v>
+      </c>
+      <c r="B136" s="2">
+        <v>18.113661504424702</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>108</v>
-      </c>
-      <c r="B137" s="1">
-        <v>13.861848774261601</v>
+        <v>98</v>
+      </c>
+      <c r="B137" s="2">
+        <v>16.658299039780598</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>109</v>
-      </c>
-      <c r="B138" s="1">
-        <v>14.153086419753038</v>
+        <v>235</v>
+      </c>
+      <c r="B138" s="2">
+        <v>29.443750000000001</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>110</v>
-      </c>
-      <c r="B139" s="1">
-        <v>15.542965023847838</v>
+        <v>236</v>
+      </c>
+      <c r="B139" s="2">
+        <v>54.365217391304341</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>111</v>
-      </c>
-      <c r="B140" s="1">
-        <v>35.121476315024395</v>
+        <v>99</v>
+      </c>
+      <c r="B140" s="2">
+        <v>10.991551347414514</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>112</v>
-      </c>
-      <c r="B141" s="1">
-        <v>11.295858378536025</v>
+        <v>100</v>
+      </c>
+      <c r="B141" s="2">
+        <v>17.643232507580347</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>113</v>
-      </c>
-      <c r="B142" s="1">
-        <v>13.363809523809531</v>
+        <v>101</v>
+      </c>
+      <c r="B142" s="2">
+        <v>24.432484076433152</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>114</v>
-      </c>
-      <c r="B143" s="1">
-        <v>24.879480519480474</v>
+        <v>102</v>
+      </c>
+      <c r="B143" s="2">
+        <v>14.61338832487306</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>115</v>
-      </c>
-      <c r="B144" s="1">
-        <v>9.4569318181819071</v>
+        <v>237</v>
+      </c>
+      <c r="B144" s="2">
+        <v>11.521875</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>116</v>
-      </c>
-      <c r="B145" s="1">
-        <v>7.3635260115605048</v>
+        <v>103</v>
+      </c>
+      <c r="B145" s="2">
+        <v>33.651175541305896</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>117</v>
-      </c>
-      <c r="B146" s="1">
-        <v>33.545765091249727</v>
+        <v>238</v>
+      </c>
+      <c r="B146" s="2">
+        <v>48.999411764705826</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>118</v>
-      </c>
-      <c r="B147" s="1">
-        <v>13.342513089005724</v>
+        <v>104</v>
+      </c>
+      <c r="B147" s="2">
+        <v>22.527391304347816</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>119</v>
-      </c>
-      <c r="B148" s="1">
-        <v>12.122222222222225</v>
+        <v>105</v>
+      </c>
+      <c r="B148" s="2">
+        <v>9.7439999999999856</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>120</v>
-      </c>
-      <c r="B149" s="1">
-        <v>11.210016155088839</v>
+        <v>106</v>
+      </c>
+      <c r="B149" s="2">
+        <v>27.022103487063973</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>121</v>
-      </c>
-      <c r="B150" s="1">
-        <v>22.758479532163751</v>
+        <v>107</v>
+      </c>
+      <c r="B150" s="2">
+        <v>13.608053055423927</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>122</v>
-      </c>
-      <c r="B151" s="1">
-        <v>19.271798460462236</v>
+        <v>239</v>
+      </c>
+      <c r="B151" s="2">
+        <v>15.866233766233767</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>123</v>
-      </c>
-      <c r="B152" s="1">
-        <v>21.312090007627678</v>
+        <v>108</v>
+      </c>
+      <c r="B152" s="2">
+        <v>14.207384665459665</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>124</v>
-      </c>
-      <c r="B153" s="1">
-        <v>43.972498160411952</v>
+        <v>109</v>
+      </c>
+      <c r="B153" s="2">
+        <v>13.889753320683084</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>125</v>
-      </c>
-      <c r="B154" s="1">
-        <v>18.412912912912951</v>
+        <v>110</v>
+      </c>
+      <c r="B154" s="2">
+        <v>16.018577140953301</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>126</v>
-      </c>
-      <c r="B155" s="1">
-        <v>19.475641025641075</v>
+        <v>111</v>
+      </c>
+      <c r="B155" s="2">
+        <v>36.065835681768526</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>127</v>
-      </c>
-      <c r="B156" s="1">
-        <v>21.294074074074064</v>
+        <v>112</v>
+      </c>
+      <c r="B156" s="2">
+        <v>11.69912414318304</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>128</v>
-      </c>
-      <c r="B157" s="1">
-        <v>31.626315789473679</v>
+        <v>113</v>
+      </c>
+      <c r="B157" s="2">
+        <v>13.65562130177516</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>129</v>
-      </c>
-      <c r="B158" s="1">
-        <v>7.6357575757575766</v>
+        <v>114</v>
+      </c>
+      <c r="B158" s="2">
+        <v>25.954929577464721</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>130</v>
-      </c>
-      <c r="B159" s="1">
-        <v>27.485936582502191</v>
+        <v>115</v>
+      </c>
+      <c r="B159" s="2">
+        <v>10.207130584192429</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>240</v>
-      </c>
-      <c r="B160" s="1">
-        <v>19.137398373983743</v>
+        <v>116</v>
+      </c>
+      <c r="B160" s="2">
+        <v>7.5872098646033104</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>131</v>
-      </c>
-      <c r="B161" s="1">
-        <v>15.369668246445521</v>
+        <v>117</v>
+      </c>
+      <c r="B161" s="2">
+        <v>34.519000000000247</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>132</v>
-      </c>
-      <c r="B162" s="1">
-        <v>14.116628440368151</v>
+        <v>118</v>
+      </c>
+      <c r="B162" s="2">
+        <v>13.487921348314909</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>133</v>
-      </c>
-      <c r="B163" s="1">
-        <v>8.4096514745308433</v>
+        <v>119</v>
+      </c>
+      <c r="B163" s="2">
+        <v>9.9400000000000031</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>134</v>
-      </c>
-      <c r="B164" s="1">
-        <v>22.484466019417468</v>
+        <v>120</v>
+      </c>
+      <c r="B164" s="2">
+        <v>13.799999999999981</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>135</v>
-      </c>
-      <c r="B165" s="1">
-        <v>42.283355300322079</v>
+        <v>121</v>
+      </c>
+      <c r="B165" s="2">
+        <v>32.749811320754709</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>136</v>
-      </c>
-      <c r="B166" s="1">
-        <v>20.487958333333456</v>
+        <v>280</v>
+      </c>
+      <c r="B166" s="2">
+        <v>14.660869565217393</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>137</v>
-      </c>
-      <c r="B167" s="1">
-        <v>16.189986468200377</v>
+        <v>122</v>
+      </c>
+      <c r="B167" s="2">
+        <v>21.670350159163242</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>241</v>
-      </c>
-      <c r="B168" s="1">
-        <v>8.934782608695647</v>
+        <v>123</v>
+      </c>
+      <c r="B168" s="2">
+        <v>22.290838709677359</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>242</v>
-      </c>
-      <c r="B169" s="1">
-        <v>26.005405405405394</v>
+        <v>124</v>
+      </c>
+      <c r="B169" s="2">
+        <v>44.982260713752105</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>138</v>
-      </c>
-      <c r="B170" s="1">
-        <v>29.932374768089666</v>
+        <v>125</v>
+      </c>
+      <c r="B170" s="2">
+        <v>19.411764705882391</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>243</v>
-      </c>
-      <c r="B171" s="1">
-        <v>3.5999999999999996</v>
+        <v>126</v>
+      </c>
+      <c r="B171" s="2">
+        <v>19.761739130434819</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>139</v>
-      </c>
-      <c r="B172" s="1">
-        <v>31.612055016182151</v>
+        <v>127</v>
+      </c>
+      <c r="B172" s="2">
+        <v>23.340370370370362</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>244</v>
-      </c>
-      <c r="B173" s="1">
-        <v>13.430769230769231</v>
+        <v>128</v>
+      </c>
+      <c r="B173" s="2">
+        <v>41.101744186046503</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>140</v>
-      </c>
-      <c r="B174" s="1">
-        <v>35.53116883116882</v>
+        <v>129</v>
+      </c>
+      <c r="B174" s="2">
+        <v>10.072608695652175</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>141</v>
-      </c>
-      <c r="B175" s="1">
-        <v>27.318935978359061</v>
+        <v>130</v>
+      </c>
+      <c r="B175" s="2">
+        <v>27.974305893814364</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>245</v>
-      </c>
-      <c r="B176" s="1">
-        <v>35.051724137931025</v>
+        <v>240</v>
+      </c>
+      <c r="B176" s="2">
+        <v>20.82134831460673</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>142</v>
-      </c>
-      <c r="B177" s="1">
-        <v>41.651685393258397</v>
+        <v>131</v>
+      </c>
+      <c r="B177" s="2">
+        <v>15.990960451977399</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>143</v>
-      </c>
-      <c r="B178" s="1">
-        <v>25.173507148864939</v>
+        <v>132</v>
+      </c>
+      <c r="B178" s="2">
+        <v>14.879998453090806</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>144</v>
-      </c>
-      <c r="B179" s="1">
-        <v>11.427910958904143</v>
+        <v>281</v>
+      </c>
+      <c r="B179" s="2">
+        <v>8.7984615384615399</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>145</v>
-      </c>
-      <c r="B180" s="1">
-        <v>25.546697365866699</v>
+        <v>133</v>
+      </c>
+      <c r="B180" s="2">
+        <v>9.6589783281733883</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>146</v>
-      </c>
-      <c r="B181" s="1">
-        <v>19.471469859620022</v>
+        <v>134</v>
+      </c>
+      <c r="B181" s="2">
+        <v>25.354822335025389</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>147</v>
-      </c>
-      <c r="B182" s="1">
-        <v>8.7254237288135545</v>
+        <v>135</v>
+      </c>
+      <c r="B182" s="2">
+        <v>43.396437418040612</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>148</v>
-      </c>
-      <c r="B183" s="1">
-        <v>16.84556962025318</v>
+        <v>136</v>
+      </c>
+      <c r="B183" s="2">
+        <v>20.8554616384917</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>149</v>
-      </c>
-      <c r="B184" s="1">
-        <v>5.7767195767195654</v>
+        <v>137</v>
+      </c>
+      <c r="B184" s="2">
+        <v>16.527974568574077</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>150</v>
-      </c>
-      <c r="B185" s="1">
-        <v>9.4136695734148805</v>
+        <v>241</v>
+      </c>
+      <c r="B185" s="2">
+        <v>8.0525423728813585</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>246</v>
-      </c>
-      <c r="B186" s="1">
-        <v>44.010810810810803</v>
+        <v>242</v>
+      </c>
+      <c r="B186" s="2">
+        <v>34.518556701030938</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>151</v>
-      </c>
-      <c r="B187" s="1">
-        <v>16.960330578512462</v>
+        <v>138</v>
+      </c>
+      <c r="B187" s="2">
+        <v>30.045891443649033</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>247</v>
-      </c>
-      <c r="B188" s="1">
-        <v>8.3582089552238763</v>
+        <v>243</v>
+      </c>
+      <c r="B188" s="2">
+        <v>11.565000000000001</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>248</v>
-      </c>
-      <c r="B189" s="1">
-        <v>18.669999999999998</v>
+        <v>139</v>
+      </c>
+      <c r="B189" s="2">
+        <v>32.239860139860866</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>152</v>
-      </c>
-      <c r="B190" s="1">
-        <v>14.945161290320932</v>
+        <v>244</v>
+      </c>
+      <c r="B190" s="2">
+        <v>18.080575539568343</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>249</v>
-      </c>
-      <c r="B191" s="1">
-        <v>13.485714285714295</v>
+        <v>140</v>
+      </c>
+      <c r="B191" s="2">
+        <v>31.025966850828734</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>153</v>
-      </c>
-      <c r="B192" s="1">
-        <v>13.478970891587773</v>
+        <v>141</v>
+      </c>
+      <c r="B192" s="2">
+        <v>29.485127478753572</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>154</v>
-      </c>
-      <c r="B193" s="1">
-        <v>25.018686868686746</v>
+        <v>245</v>
+      </c>
+      <c r="B193" s="2">
+        <v>58.200000000000031</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>250</v>
-      </c>
-      <c r="B194" s="1">
-        <v>22.32</v>
+        <v>142</v>
+      </c>
+      <c r="B194" s="2">
+        <v>41.909694555112871</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>155</v>
-      </c>
-      <c r="B195" s="1">
-        <v>11.267727380670301</v>
+        <v>143</v>
+      </c>
+      <c r="B195" s="2">
+        <v>26.266826295167238</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>156</v>
-      </c>
-      <c r="B196" s="1">
-        <v>10.222994652406337</v>
+        <v>144</v>
+      </c>
+      <c r="B196" s="2">
+        <v>12.19416983523452</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>157</v>
-      </c>
-      <c r="B197" s="1">
-        <v>15.984615384615385</v>
+        <v>145</v>
+      </c>
+      <c r="B197" s="2">
+        <v>26.320615263470103</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>158</v>
-      </c>
-      <c r="B198" s="1">
-        <v>41.358018867924628</v>
+        <v>146</v>
+      </c>
+      <c r="B198" s="2">
+        <v>20.298571428570998</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>159</v>
-      </c>
-      <c r="B199" s="1">
-        <v>12.114838129496389</v>
+        <v>147</v>
+      </c>
+      <c r="B199" s="2">
+        <v>9.113333333333328</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>160</v>
-      </c>
-      <c r="B200" s="1">
-        <v>9.6733027522938428</v>
+        <v>148</v>
+      </c>
+      <c r="B200" s="2">
+        <v>26.91547619047623</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>161</v>
-      </c>
-      <c r="B201" s="1">
-        <v>9.3629151291514443</v>
+        <v>149</v>
+      </c>
+      <c r="B201" s="2">
+        <v>7.1139534883720987</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>162</v>
-      </c>
-      <c r="B202" s="1">
-        <v>12.936102236421801</v>
+        <v>282</v>
+      </c>
+      <c r="B202" s="2">
+        <v>56.276470588235306</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>163</v>
-      </c>
-      <c r="B203" s="1">
-        <v>33.035359143040054</v>
+        <v>150</v>
+      </c>
+      <c r="B203" s="2">
+        <v>9.5686370099532319</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>251</v>
-      </c>
-      <c r="B204" s="1">
-        <v>25.860869565217396</v>
+        <v>246</v>
+      </c>
+      <c r="B204" s="2">
+        <v>50.644999999999989</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>164</v>
-      </c>
-      <c r="B205" s="1">
-        <v>40.643200000000014</v>
+        <v>151</v>
+      </c>
+      <c r="B205" s="2">
+        <v>17.638264299802817</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>165</v>
-      </c>
-      <c r="B206" s="1">
-        <v>22.767105263157916</v>
+        <v>247</v>
+      </c>
+      <c r="B206" s="2">
+        <v>7.8985454545454692</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>252</v>
-      </c>
-      <c r="B207" s="1">
-        <v>6.7200000000000033</v>
+        <v>248</v>
+      </c>
+      <c r="B207" s="2">
+        <v>19.328947368421062</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>253</v>
-      </c>
-      <c r="B208" s="1">
-        <v>57.608333333333313</v>
+        <v>152</v>
+      </c>
+      <c r="B208" s="2">
+        <v>15.157272481770185</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>166</v>
-      </c>
-      <c r="B209" s="1">
-        <v>23.096774193548146</v>
+        <v>283</v>
+      </c>
+      <c r="B209" s="2">
+        <v>13.033333333333333</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>167</v>
-      </c>
-      <c r="B210" s="1">
-        <v>18.412950819671718</v>
+        <v>249</v>
+      </c>
+      <c r="B210" s="2">
+        <v>13.604255319148942</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>168</v>
-      </c>
-      <c r="B211" s="1">
-        <v>22.850488599348644</v>
+        <v>153</v>
+      </c>
+      <c r="B211" s="2">
+        <v>13.612859034426972</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>254</v>
-      </c>
-      <c r="B212" s="1">
-        <v>8.4121212121212139</v>
+        <v>154</v>
+      </c>
+      <c r="B212" s="2">
+        <v>26.496830427892153</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>169</v>
-      </c>
-      <c r="B213" s="1">
-        <v>13.417656765676247</v>
+        <v>250</v>
+      </c>
+      <c r="B213" s="2">
+        <v>23.088709677419352</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>170</v>
-      </c>
-      <c r="B214" s="1">
-        <v>18.616630901287547</v>
+        <v>155</v>
+      </c>
+      <c r="B214" s="2">
+        <v>11.433320165909945</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>171</v>
-      </c>
-      <c r="B215" s="1">
-        <v>19.447848506401034</v>
+        <v>156</v>
+      </c>
+      <c r="B215" s="2">
+        <v>11.135443037974621</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>172</v>
-      </c>
-      <c r="B216" s="1">
-        <v>16.279148936170238</v>
+        <v>284</v>
+      </c>
+      <c r="B216" s="2">
+        <v>21.182352941176468</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>255</v>
-      </c>
-      <c r="B217" s="1">
-        <v>10.137272727272734</v>
+        <v>157</v>
+      </c>
+      <c r="B217" s="2">
+        <v>15.945945945945946</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>173</v>
-      </c>
-      <c r="B218" s="1">
-        <v>30.896183206106848</v>
+        <v>158</v>
+      </c>
+      <c r="B218" s="2">
+        <v>48.303448275862117</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>174</v>
-      </c>
-      <c r="B219" s="1">
-        <v>24.52737430167598</v>
+        <v>159</v>
+      </c>
+      <c r="B219" s="2">
+        <v>13.430704493009848</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>175</v>
-      </c>
-      <c r="B220" s="1">
-        <v>27.17792207792213</v>
+        <v>160</v>
+      </c>
+      <c r="B220" s="2">
+        <v>10.208237105465869</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>176</v>
-      </c>
-      <c r="B221" s="1">
-        <v>14.434007274282354</v>
+        <v>161</v>
+      </c>
+      <c r="B221" s="2">
+        <v>9.5521881123449504</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>177</v>
-      </c>
-      <c r="B222" s="1">
-        <v>12.396598639455762</v>
+        <v>162</v>
+      </c>
+      <c r="B222" s="2">
+        <v>14.402252252252254</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>178</v>
-      </c>
-      <c r="B223" s="1">
-        <v>5.9233676975945428</v>
+        <v>163</v>
+      </c>
+      <c r="B223" s="2">
+        <v>34.697673000921959</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>179</v>
-      </c>
-      <c r="B224" s="1">
-        <v>11.617894736842091</v>
+        <v>251</v>
+      </c>
+      <c r="B224" s="2">
+        <v>25.442647058823532</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>180</v>
-      </c>
-      <c r="B225" s="1">
-        <v>14.233345033345195</v>
+        <v>164</v>
+      </c>
+      <c r="B225" s="2">
+        <v>40.463874345549748</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>256</v>
-      </c>
-      <c r="B226" s="1">
-        <v>10.068000000000001</v>
+        <v>165</v>
+      </c>
+      <c r="B226" s="2">
+        <v>21.028358208955247</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>257</v>
-      </c>
-      <c r="B227" s="1">
-        <v>10.042253521126753</v>
+        <v>252</v>
+      </c>
+      <c r="B227" s="2">
+        <v>6.3435897435897459</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>181</v>
-      </c>
-      <c r="B228" s="1">
-        <v>12.846348476135542</v>
+        <v>253</v>
+      </c>
+      <c r="B228" s="2">
+        <v>53.277192982456135</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>182</v>
-      </c>
-      <c r="B229" s="1">
-        <v>15.592139554434731</v>
+        <v>166</v>
+      </c>
+      <c r="B229" s="2">
+        <v>24.459152215799435</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>183</v>
-      </c>
-      <c r="B230" s="1">
-        <v>25.667229729730309</v>
+        <v>167</v>
+      </c>
+      <c r="B230" s="2">
+        <v>20.902644230768903</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>184</v>
-      </c>
-      <c r="B231" s="1">
-        <v>14.521951219512216</v>
+        <v>285</v>
+      </c>
+      <c r="B231" s="2">
+        <v>26.32</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>185</v>
-      </c>
-      <c r="B232" s="1">
-        <v>31.113611111111105</v>
+        <v>168</v>
+      </c>
+      <c r="B232" s="2">
+        <v>24.361276595744737</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>186</v>
-      </c>
-      <c r="B233" s="1">
-        <v>24.875627240143469</v>
+        <v>254</v>
+      </c>
+      <c r="B233" s="2">
+        <v>10.171875000000005</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>187</v>
-      </c>
-      <c r="B234" s="1">
-        <v>13.9427272727273</v>
+        <v>169</v>
+      </c>
+      <c r="B234" s="2">
+        <v>13.353654024051645</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>188</v>
-      </c>
-      <c r="B235" s="1">
-        <v>8.6270501835986462</v>
+        <v>170</v>
+      </c>
+      <c r="B235" s="2">
+        <v>19.406203473945386</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>189</v>
-      </c>
-      <c r="B236" s="1">
-        <v>29.281666666666641</v>
+        <v>171</v>
+      </c>
+      <c r="B236" s="2">
+        <v>19.991503748345206</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>258</v>
-      </c>
-      <c r="B237" s="1">
-        <v>13.695348837209307</v>
+        <v>172</v>
+      </c>
+      <c r="B237" s="2">
+        <v>17.440816326530634</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>190</v>
-      </c>
-      <c r="B238" s="1">
-        <v>7.2241379310344387</v>
+        <v>255</v>
+      </c>
+      <c r="B238" s="2">
+        <v>9.4615120274913789</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>191</v>
-      </c>
-      <c r="B239" s="1">
-        <v>21.822054263566372</v>
+        <v>173</v>
+      </c>
+      <c r="B239" s="2">
+        <v>33.756249999999952</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>192</v>
-      </c>
-      <c r="B240" s="1">
-        <v>25.175971370143003</v>
+        <v>174</v>
+      </c>
+      <c r="B240" s="2">
+        <v>28.049538461538475</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>193</v>
-      </c>
-      <c r="B241" s="1">
-        <v>10.847924196543657</v>
+        <v>175</v>
+      </c>
+      <c r="B241" s="2">
+        <v>36.461575178997727</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>259</v>
-      </c>
-      <c r="B242" s="1">
-        <v>17.349999999999998</v>
+        <v>176</v>
+      </c>
+      <c r="B242" s="2">
+        <v>14.53810182095407</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>194</v>
-      </c>
-      <c r="B243" s="1">
-        <v>11.210696266397722</v>
+        <v>177</v>
+      </c>
+      <c r="B243" s="2">
+        <v>12.779534883720926</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>195</v>
-      </c>
-      <c r="B244" s="1">
-        <v>12.170617283950648</v>
+        <v>178</v>
+      </c>
+      <c r="B244" s="2">
+        <v>6.1291581108829689</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>260</v>
-      </c>
-      <c r="B245" s="1">
-        <v>30.383333333333351</v>
+        <v>179</v>
+      </c>
+      <c r="B245" s="2">
+        <v>10.948880597014917</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>196</v>
-      </c>
-      <c r="B246" s="1">
-        <v>25.576307363927484</v>
+        <v>180</v>
+      </c>
+      <c r="B246" s="2">
+        <v>14.545802432512753</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>261</v>
-      </c>
-      <c r="B247" s="1">
-        <v>12.472222222222225</v>
+        <v>256</v>
+      </c>
+      <c r="B247" s="2">
+        <v>11.780503144654096</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>197</v>
-      </c>
-      <c r="B248" s="1">
-        <v>28.592678227360238</v>
+        <v>257</v>
+      </c>
+      <c r="B248" s="2">
+        <v>12.116756756756743</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>198</v>
-      </c>
-      <c r="B249" s="1">
-        <v>11.885350122851543</v>
+        <v>181</v>
+      </c>
+      <c r="B249" s="2">
+        <v>12.857135826771605</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>262</v>
-      </c>
-      <c r="B250" s="1">
-        <v>22.666666666666668</v>
+        <v>182</v>
+      </c>
+      <c r="B250" s="2">
+        <v>16.77424042272137</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>263</v>
-      </c>
-      <c r="B251" s="1">
-        <v>14.299999999999995</v>
+        <v>183</v>
+      </c>
+      <c r="B251" s="2">
+        <v>25.664686468647162</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>199</v>
-      </c>
-      <c r="B252" s="1">
-        <v>34.81396620278317</v>
+        <v>184</v>
+      </c>
+      <c r="B252" s="2">
+        <v>14.243925233644889</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>200</v>
-      </c>
-      <c r="B253" s="1">
-        <v>24.041176470588201</v>
+        <v>185</v>
+      </c>
+      <c r="B253" s="2">
+        <v>30.810515021459221</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>201</v>
-      </c>
-      <c r="B254" s="1">
-        <v>20.979597233524157</v>
+        <v>186</v>
+      </c>
+      <c r="B254" s="2">
+        <v>32.986111111111036</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>202</v>
-      </c>
-      <c r="B255" s="1">
-        <v>10.67035398230111</v>
+        <v>187</v>
+      </c>
+      <c r="B255" s="2">
+        <v>14.078983516483529</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>203</v>
-      </c>
-      <c r="B256" s="1">
-        <v>10.235890557939967</v>
+        <v>188</v>
+      </c>
+      <c r="B256" s="2">
+        <v>8.803327171903959</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>204</v>
-      </c>
-      <c r="B257" s="1">
-        <v>33.522169811320744</v>
+        <v>189</v>
+      </c>
+      <c r="B257" s="2">
+        <v>32.744230769230768</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>264</v>
-      </c>
-      <c r="B258" s="1">
-        <v>8.4090909090909083</v>
+        <v>258</v>
+      </c>
+      <c r="B258" s="2">
+        <v>13.541573033707875</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>205</v>
-      </c>
-      <c r="B259" s="1">
-        <v>7.422448979591854</v>
+        <v>190</v>
+      </c>
+      <c r="B259" s="2">
+        <v>8.0706666666666305</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>206</v>
-      </c>
-      <c r="B260" s="1">
-        <v>20.130000000000074</v>
+        <v>191</v>
+      </c>
+      <c r="B260" s="2">
+        <v>22.264493712773398</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>207</v>
-      </c>
-      <c r="B261" s="1">
-        <v>11.042957746479113</v>
+        <v>192</v>
+      </c>
+      <c r="B261" s="2">
+        <v>25.508703819661747</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>208</v>
-      </c>
-      <c r="B262" s="1">
-        <v>11.481772508038786</v>
+        <v>193</v>
+      </c>
+      <c r="B262" s="2">
+        <v>11.20550245414732</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>209</v>
-      </c>
-      <c r="B263" s="1">
-        <v>11.341996233521545</v>
+        <v>259</v>
+      </c>
+      <c r="B263" s="2">
+        <v>23.690476190476186</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
+        <v>194</v>
+      </c>
+      <c r="B264" s="2">
+        <v>10.626746849942826</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
+        <v>195</v>
+      </c>
+      <c r="B265" s="2">
+        <v>13.587991021324344</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
+        <v>260</v>
+      </c>
+      <c r="B266" s="2">
+        <v>55.11297872340446</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
+        <v>286</v>
+      </c>
+      <c r="B267" s="2">
+        <v>64.196498054474674</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
+        <v>196</v>
+      </c>
+      <c r="B268" s="2">
+        <v>24.460278207109802</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
+        <v>261</v>
+      </c>
+      <c r="B269" s="2">
+        <v>14.620895522388055</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
+        <v>287</v>
+      </c>
+      <c r="B270" s="2">
+        <v>18.562499999999996</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A271" t="s">
+        <v>197</v>
+      </c>
+      <c r="B271" s="2">
+        <v>28.491916167664613</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A272" t="s">
+        <v>198</v>
+      </c>
+      <c r="B272" s="2">
+        <v>12.108649917413857</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A273" t="s">
+        <v>262</v>
+      </c>
+      <c r="B273" s="2">
+        <v>48.484331797234944</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
+        <v>263</v>
+      </c>
+      <c r="B274" s="2">
+        <v>15.355357142857144</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A275" t="s">
+        <v>199</v>
+      </c>
+      <c r="B275" s="2">
+        <v>37.492808478425317</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A276" t="s">
+        <v>200</v>
+      </c>
+      <c r="B276" s="2">
+        <v>24.238474870017335</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A277" t="s">
+        <v>201</v>
+      </c>
+      <c r="B277" s="2">
+        <v>21.23203849518854</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A278" t="s">
+        <v>202</v>
+      </c>
+      <c r="B278" s="2">
+        <v>11.223235800344419</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A279" t="s">
+        <v>203</v>
+      </c>
+      <c r="B279" s="2">
+        <v>10.204266211604102</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A280" t="s">
+        <v>204</v>
+      </c>
+      <c r="B280" s="2">
+        <v>35.174999999999983</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A281" t="s">
+        <v>264</v>
+      </c>
+      <c r="B281" s="2">
+        <v>11.447222222222235</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A282" t="s">
+        <v>205</v>
+      </c>
+      <c r="B282" s="2">
+        <v>8.0422053231939366</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
+        <v>206</v>
+      </c>
+      <c r="B283" s="2">
+        <v>15.741054313099076</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A284" t="s">
+        <v>207</v>
+      </c>
+      <c r="B284" s="2">
+        <v>11.180102915952153</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A285" t="s">
+        <v>208</v>
+      </c>
+      <c r="B285" s="2">
+        <v>11.648359788360064</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A286" t="s">
+        <v>209</v>
+      </c>
+      <c r="B286" s="2">
+        <v>10.644895104895049</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A287" t="s">
         <v>210</v>
       </c>
-      <c r="B264" s="1">
-        <v>32.940226171243921</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A265" s="2"/>
-      <c r="B265" s="3"/>
+      <c r="B287" s="2">
+        <v>33.659318423855012</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A288" s="1"/>
+      <c r="B288" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>